<commit_message>
added team11 to sheet
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre van der Hoek\Desktop\SWE 265P\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\SWE265\W2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FB1BA0D-4D38-45E0-9F49-B787D7DB1A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F9AA25B-4FEB-498C-BC59-B613A262BA0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="86280" yWindow="-120" windowWidth="29040" windowHeight="17790" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{0CF5F261-EB17-4B41-A711-49E3E5ABBDDE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="35">
   <si>
     <t>TEAMS</t>
   </si>
@@ -90,12 +90,6 @@
     <t>Team 11</t>
   </si>
   <si>
-    <t>&lt;member #4 name&gt;</t>
-  </si>
-  <si>
-    <t>&lt;member #4 e-mail&gt;</t>
-  </si>
-  <si>
     <t>&lt;member #1 github id&gt;</t>
   </si>
   <si>
@@ -105,14 +99,50 @@
     <t>&lt;member #3 github id&gt;</t>
   </si>
   <si>
-    <t>&lt;member #4 github id&gt;</t>
+    <t>Git Good</t>
+  </si>
+  <si>
+    <t>Rafael Oliveira</t>
+  </si>
+  <si>
+    <t>rcortezb@uci.edu</t>
+  </si>
+  <si>
+    <t>rafbel</t>
+  </si>
+  <si>
+    <t>Hyun Jay Yang</t>
+  </si>
+  <si>
+    <t>hjyang1@uci.edu</t>
+  </si>
+  <si>
+    <t>hjayyang94</t>
+  </si>
+  <si>
+    <t>Nicolas Grantham</t>
+  </si>
+  <si>
+    <t>ngrantha@uci.edu</t>
+  </si>
+  <si>
+    <t>GranthamAnthem</t>
+  </si>
+  <si>
+    <t>Chris Zhang</t>
+  </si>
+  <si>
+    <t>czhang29@uci.edu</t>
+  </si>
+  <si>
+    <t>ch-zha</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,6 +188,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -186,12 +224,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -202,9 +241,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -520,16 +561,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03ADA9CD-54FE-4929-A60C-E962D9D8534C}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="7" width="34.6328125" customWidth="1"/>
+    <col min="1" max="7" width="34.62890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -540,7 +581,7 @@
       <c r="F1" s="5"/>
       <c r="G1" s="5"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -549,7 +590,7 @@
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -572,7 +613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -595,7 +636,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -604,7 +645,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -627,7 +668,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
@@ -650,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -673,7 +714,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
@@ -696,7 +737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -719,7 +760,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -742,76 +783,76 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="A14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -820,7 +861,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -829,7 +870,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A17" s="4" t="s">
         <v>15</v>
       </c>
@@ -846,7 +887,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
@@ -857,13 +898,13 @@
         <v>8</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -872,7 +913,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A20" s="3" t="s">
         <v>9</v>
       </c>
@@ -883,13 +924,13 @@
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A21" s="3" t="s">
         <v>10</v>
       </c>
@@ -900,13 +941,13 @@
         <v>10</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
@@ -917,13 +958,13 @@
         <v>11</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A23" s="3" t="s">
         <v>12</v>
       </c>
@@ -934,13 +975,13 @@
         <v>12</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A24" s="3" t="s">
         <v>14</v>
       </c>
@@ -950,14 +991,14 @@
       <c r="C24" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>12</v>
+      <c r="D24" s="6" t="s">
+        <v>24</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A25" s="3" t="s">
         <v>13</v>
       </c>
@@ -967,98 +1008,98 @@
       <c r="C25" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="3" t="s">
-        <v>14</v>
+      <c r="D25" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A27" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="3" t="s">
         <v>20</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>33</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A28" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.6">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1071,7 +1112,13 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D24" r:id="rId1" xr:uid="{FDAEED22-3133-427E-92EF-9E07DF9894DA}"/>
+    <hyperlink ref="D25" r:id="rId2" xr:uid="{8FEA37F2-F653-4584-A1A5-6F36CCA9A272}"/>
+    <hyperlink ref="D26" r:id="rId3" xr:uid="{D67CDDBD-E73F-430E-BC9A-AF739ABA7E9A}"/>
+    <hyperlink ref="D27" r:id="rId4" xr:uid="{E4848063-3439-4C36-942C-2C1FCAB80046}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved Merge Conflicts for #25 (#28)
* Add files via upload

* Add files via upload

* Add files via upload

* Add files via upload

* Delete Bulter.sh

* upload

* test

* test

* Merged master content in here and fixed project directory.

Co-authored-by: Danny7226 <duochai9611@gmail.com>
Co-authored-by: Kaj Dreef <kaj.dreef@gmail.com>
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="55">
   <si>
     <t xml:space="preserve">TEAMS</t>
   </si>
@@ -49,58 +49,88 @@
     <t xml:space="preserve">Work, work</t>
   </si>
   <si>
+    <t xml:space="preserve">Team_Costco</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;team name&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Dongxin Xiang</t>
   </si>
   <si>
+    <t xml:space="preserve">Marc Andrada</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #1 name&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Jing Chen</t>
   </si>
   <si>
+    <t xml:space="preserve">Soobin Choi</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #2 name&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Guowei Li</t>
   </si>
   <si>
+    <t xml:space="preserve">Duo Chai</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #3 name&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">dongxix@uci.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">andradam@uci.edu</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #1 e-mail&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">anniejingchen@gmail.com</t>
   </si>
   <si>
+    <t xml:space="preserve">soobinc3@uci.edu</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #2 e-mail&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">guowel2@uci.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">dchai2@uci.edu</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #3 e-mail&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">sunflower0309</t>
   </si>
   <si>
+    <t xml:space="preserve">nbalumpia</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #1 github id&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">anniejingchen</t>
   </si>
   <si>
+    <t xml:space="preserve">soobinchoi54</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #2 github id&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">oscarli9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Danny7226</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;member #3 github id&gt;</t>
@@ -231,6 +261,7 @@
       <color rgb="FF0000FF"/>
       <name val="等线"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -443,11 +474,11 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D18:D31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="34.63"/>
   </cols>
@@ -503,19 +534,19 @@
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,211 +558,211 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="5" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -754,16 +785,16 @@
     </row>
     <row r="17" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -771,16 +802,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -797,16 +828,16 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -814,16 +845,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -831,16 +862,16 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
@@ -848,16 +879,16 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
@@ -865,16 +896,16 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -882,16 +913,16 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
@@ -899,16 +930,16 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -916,16 +947,16 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -933,16 +964,16 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
@@ -953,7 +984,7 @@
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="7" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
@@ -964,7 +995,7 @@
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="7" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
@@ -975,7 +1006,7 @@
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="7" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -996,12 +1027,15 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A9" r:id="rId1" display="dongxix@uci.edu"/>
-    <hyperlink ref="A10" r:id="rId2" display="anniejingchen@gmail.com"/>
-    <hyperlink ref="A11" r:id="rId3" display="guowel2@uci.edu"/>
-    <hyperlink ref="D24" r:id="rId4" display="rcortezb@uci.edu"/>
-    <hyperlink ref="D25" r:id="rId5" display="hjyang1@uci.edu"/>
-    <hyperlink ref="D26" r:id="rId6" display="ngrantha@uci.edu"/>
-    <hyperlink ref="D27" r:id="rId7" display="czhang29@uci.edu"/>
+    <hyperlink ref="B9" r:id="rId2" display="andradam@uci.edu"/>
+    <hyperlink ref="A10" r:id="rId3" display="anniejingchen@gmail.com"/>
+    <hyperlink ref="B10" r:id="rId4" display="soobinc3@uci.edu"/>
+    <hyperlink ref="A11" r:id="rId5" display="guowel2@uci.edu"/>
+    <hyperlink ref="B11" r:id="rId6" display="dchai2@uci.edu"/>
+    <hyperlink ref="D24" r:id="rId7" display="rcortezb@uci.edu"/>
+    <hyperlink ref="D25" r:id="rId8" display="hjyang1@uci.edu"/>
+    <hyperlink ref="D26" r:id="rId9" display="ngrantha@uci.edu"/>
+    <hyperlink ref="D27" r:id="rId10" display="czhang29@uci.edu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
added diaries/diary-junxian-chen.xlsx and our team
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yorkson/Dropbox/MSWE-Q2/SWE 265P/my_W2020/W2020/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joxon\Documents\_Repos\swe265p-reveng\W2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72C8C21-52BF-8345-B327-69F447E53077}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341AF98B-D411-40C8-B3F4-D3367A72ADF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -252,42 +252,42 @@
     <t>ch-zha</t>
   </si>
   <si>
-    <t>Skateboard2Wheelchair</t>
+    <t>Junxian Chen</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>Yue Zhang</t>
+    <t>Wen Chia Yang</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>Zeyu Huang</t>
+    <t>Zihua Weng</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>Tianlun Li</t>
+    <t>junxiac1@uci.edu</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>zeyuh10@uci.edu</t>
+    <t>joxon</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>yue.zhang@uci.edu</t>
+    <t>Solution Accepted</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>tianlul3@uci.edu</t>
+    <t>zihuaw2@uci.edu</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>YorksonChang</t>
+    <t>zihuaweng</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
   <si>
-    <t>ShawnLi1014</t>
-  </si>
-  <si>
-    <t>Zeyuuuuuu</t>
+    <t>wenchiayang</t>
+  </si>
+  <si>
+    <t>wcyang1@uci.edu</t>
     <phoneticPr fontId="10" type="noConversion"/>
   </si>
 </sst>
@@ -295,7 +295,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -369,7 +369,6 @@
     <font>
       <sz val="9"/>
       <name val="等线"/>
-      <family val="4"/>
       <charset val="134"/>
     </font>
     <font>
@@ -377,7 +376,7 @@
       <sz val="12"/>
       <color rgb="FF9C5700"/>
       <name val="等线"/>
-      <family val="4"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -416,7 +415,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -432,12 +431,13 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Bad" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -521,7 +521,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -820,15 +820,15 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,7 +839,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1">
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -848,7 +848,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="16">
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -871,7 +871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="16">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -890,11 +890,11 @@
       <c r="F4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="16">
+      <c r="G4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -903,7 +903,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="16">
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -922,11 +922,11 @@
       <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="16">
+      <c r="G6" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -945,11 +945,11 @@
       <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="16">
+      <c r="G7" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -968,11 +968,11 @@
       <c r="F8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16">
+      <c r="G8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -992,10 +992,10 @@
         <v>27</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>28</v>
       </c>
@@ -1015,10 +1015,10 @@
         <v>31</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="16">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>32</v>
       </c>
@@ -1038,10 +1038,10 @@
         <v>35</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>36</v>
       </c>
@@ -1060,11 +1060,11 @@
       <c r="F12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="16">
+      <c r="G12" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>40</v>
       </c>
@@ -1083,11 +1083,11 @@
       <c r="F13" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="16">
+      <c r="G13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>44</v>
       </c>
@@ -1107,10 +1107,10 @@
         <v>47</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1119,7 +1119,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" ht="16">
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1128,7 +1128,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="1:7" ht="16">
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
@@ -1145,15 +1145,15 @@
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="1:7" ht="16">
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>11</v>
+      <c r="C18" s="10" t="s">
+        <v>80</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>53</v>
@@ -1162,7 +1162,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" ht="16">
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1171,15 +1171,15 @@
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:7" ht="16">
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>15</v>
+      <c r="C20" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>55</v>
@@ -1188,15 +1188,15 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="16">
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>19</v>
+      <c r="C21" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="D21" s="7" t="s">
         <v>57</v>
@@ -1205,15 +1205,15 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" ht="16">
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>23</v>
+      <c r="C22" s="10" t="s">
+        <v>77</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>59</v>
@@ -1222,15 +1222,15 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="16">
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>27</v>
+      <c r="C23" s="11" t="s">
+        <v>78</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>61</v>
@@ -1239,15 +1239,15 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" ht="16">
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>31</v>
+      <c r="C24" s="11" t="s">
+        <v>84</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>63</v>
@@ -1256,15 +1256,15 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" ht="16">
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>35</v>
+      <c r="C25" s="11" t="s">
+        <v>81</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>65</v>
@@ -1273,15 +1273,15 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="16">
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>66</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>39</v>
+      <c r="C26" s="10" t="s">
+        <v>79</v>
       </c>
       <c r="D26" s="9" t="s">
         <v>67</v>
@@ -1290,7 +1290,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" ht="16">
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>68</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>43</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="D27" s="9" t="s">
         <v>69</v>
@@ -1307,15 +1307,15 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" ht="16">
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>47</v>
+      <c r="C28" s="10" t="s">
+        <v>82</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>71</v>
@@ -1324,7 +1324,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" ht="16">
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -1335,7 +1335,7 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" ht="16">
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1346,7 +1346,7 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" ht="16">
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1357,7 +1357,7 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" ht="16">
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1388,11 +1388,11 @@
     <hyperlink ref="D25" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
     <hyperlink ref="D26" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="D27" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="G10" r:id="rId17" xr:uid="{F93FAF08-6C1E-CF4E-AE23-6DF8E2EA8B7A}"/>
-    <hyperlink ref="G11" r:id="rId18" xr:uid="{164C78FD-80FA-4B42-ABDD-24F5AD92BA12}"/>
-    <hyperlink ref="G9" r:id="rId19" xr:uid="{462FC0CF-D320-194A-8439-4BA2C87999CE}"/>
+    <hyperlink ref="C23" r:id="rId17" xr:uid="{5A0E23D5-E35A-4B07-A4F9-B55C4E2F6EC7}"/>
+    <hyperlink ref="C25" r:id="rId18" xr:uid="{21AC8A0A-38BE-4100-A5FC-669C40FBBB4C}"/>
+    <hyperlink ref="C24" r:id="rId19" xr:uid="{B2820CA6-18D6-48B6-A3AF-3834F292398B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
re-added missing info for team 7 (Sorry :)
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -8,24 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joxon\Documents\_Repos\swe265p-reveng\W2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{341AF98B-D411-40C8-B3F4-D3367A72ADF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33326936-684A-4DEE-95F6-5258EAB12548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11148" yWindow="2232" windowWidth="17280" windowHeight="10044" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
   <si>
     <t>TEAMS</t>
   </si>
@@ -289,13 +284,43 @@
   <si>
     <t>wcyang1@uci.edu</t>
     <phoneticPr fontId="10" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skateboard2Wheelchair</t>
+  </si>
+  <si>
+    <t>Yue Zhang</t>
+  </si>
+  <si>
+    <t>Zeyu Huang</t>
+  </si>
+  <si>
+    <t>Tianlun Li</t>
+  </si>
+  <si>
+    <t>yue.zhang@uci.edu</t>
+  </si>
+  <si>
+    <t>zeyuh10@uci.edu</t>
+  </si>
+  <si>
+    <t>tianlul3@uci.edu</t>
+  </si>
+  <si>
+    <t>YorksonChang</t>
+  </si>
+  <si>
+    <t>Zeyuuuuuu</t>
+  </si>
+  <si>
+    <t>ShawnLi1014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -379,6 +404,14 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -415,11 +448,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -432,6 +462,12 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Bad" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -819,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -829,542 +865,542 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
     </row>
     <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="13"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="5"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="C18" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
+      <c r="C20" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="C21" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="3" t="s">
+      <c r="C22" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="C23" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" s="3" t="s">
+      <c r="C24" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="3" t="s">
+      <c r="C25" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="3" t="s">
+      <c r="C26" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="C27" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="7" t="s">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="7" t="s">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="7" t="s">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A32" s="4"/>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="6"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1391,8 +1427,11 @@
     <hyperlink ref="C23" r:id="rId17" xr:uid="{5A0E23D5-E35A-4B07-A4F9-B55C4E2F6EC7}"/>
     <hyperlink ref="C25" r:id="rId18" xr:uid="{21AC8A0A-38BE-4100-A5FC-669C40FBBB4C}"/>
     <hyperlink ref="C24" r:id="rId19" xr:uid="{B2820CA6-18D6-48B6-A3AF-3834F292398B}"/>
+    <hyperlink ref="G10" r:id="rId20" xr:uid="{F93FAF08-6C1E-CF4E-AE23-6DF8E2EA8B7A}"/>
+    <hyperlink ref="G11" r:id="rId21" xr:uid="{164C78FD-80FA-4B42-ABDD-24F5AD92BA12}"/>
+    <hyperlink ref="G9" r:id="rId22" xr:uid="{462FC0CF-D320-194A-8439-4BA2C87999CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId20"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId23"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated team member information
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joxon\Documents\_Repos\swe265p-reveng\W2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Marc/Desktop/W2020/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33326936-684A-4DEE-95F6-5258EAB12548}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280289DD-D270-5B44-9855-09F9A584AD7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11148" yWindow="2232" windowWidth="17280" windowHeight="10044" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4760" yWindow="2180" windowWidth="17280" windowHeight="10040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -133,9 +133,6 @@
     <t>sunflower0309</t>
   </si>
   <si>
-    <t>nbalumpia</t>
-  </si>
-  <si>
     <t>aman-bhatia94</t>
   </si>
   <si>
@@ -314,13 +311,16 @@
   </si>
   <si>
     <t>ShawnLi1014</t>
+  </si>
+  <si>
+    <t>marc-andrada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -462,12 +462,12 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Bad" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
@@ -855,36 +855,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:7" ht="21" customHeight="1">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="16">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -907,7 +907,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="16">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -926,20 +926,20 @@
       <c r="F4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G4" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="16">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="13"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="16">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -958,11 +958,11 @@
       <c r="F6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G6" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -981,11 +981,11 @@
       <c r="F7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G7" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16">
       <c r="A8" s="2" t="s">
         <v>20</v>
       </c>
@@ -1004,11 +1004,11 @@
       <c r="F8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G8" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="16">
       <c r="A9" s="4" t="s">
         <v>24</v>
       </c>
@@ -1027,11 +1027,11 @@
       <c r="F9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G9" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="16">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -1050,11 +1050,11 @@
       <c r="F10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G10" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16">
       <c r="A11" s="4" t="s">
         <v>32</v>
       </c>
@@ -1073,80 +1073,80 @@
       <c r="F11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G11" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="16">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="16">
+      <c r="A13" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="14" t="s">
+      <c r="B13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="2" t="s">
+    <row r="14" spans="1:7" ht="16">
+      <c r="A14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="14" t="s">
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="11" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="16">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1155,7 +1155,7 @@
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
     </row>
-    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="16">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1164,41 +1164,41 @@
       <c r="F16" s="3"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="16">
       <c r="A17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="16">
       <c r="A18" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="16">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1207,193 +1207,193 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16">
       <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="16">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="16">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="16">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="16">
       <c r="A24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="16">
       <c r="A25" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="16">
       <c r="A26" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>66</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>67</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="16">
       <c r="A27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>68</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>69</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="16">
       <c r="A28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="6" t="s">
         <v>70</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>71</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="16">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="16">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="16">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="16">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>

</xml_diff>

<commit_message>
Resolve merge conflict of PR42 (#54) Close #42
* diary added

* team added - Yijia, Bingfei, Xiling

* Added project folder to the repo for team Foobar.

Co-authored-by: Xiling <52394061+xilingl1@users.noreply.github.com>
Co-authored-by: Kaj Dreef <kaj.dreef@gmail.com>
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
   <si>
     <t xml:space="preserve">TEAMS</t>
   </si>
@@ -55,6 +55,9 @@
     <t xml:space="preserve">Runtime Terror</t>
   </si>
   <si>
+    <t xml:space="preserve">Foobar</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;team name&gt;</t>
   </si>
   <si>
@@ -70,6 +73,9 @@
     <t xml:space="preserve">Aman Bhatia</t>
   </si>
   <si>
+    <t xml:space="preserve">Yijia Zhang</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #1 name&gt;</t>
   </si>
   <si>
@@ -85,6 +91,9 @@
     <t xml:space="preserve">Anjana Krishnakumar Vellore</t>
   </si>
   <si>
+    <t xml:space="preserve">Bingfei Zhang</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #2 name&gt;</t>
   </si>
   <si>
@@ -100,6 +109,9 @@
     <t xml:space="preserve">Vaishakhi Pilankar</t>
   </si>
   <si>
+    <t xml:space="preserve">Xiling Li</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #3 name&gt;</t>
   </si>
   <si>
@@ -115,6 +127,9 @@
     <t xml:space="preserve">amanb1@uci.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">yijiz13@uci.edu</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #1 e-mail&gt;</t>
   </si>
   <si>
@@ -130,6 +145,9 @@
     <t xml:space="preserve">anjanak1@uci.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">bingfeiz@uci.edu</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #2 e-mail&gt;</t>
   </si>
   <si>
@@ -145,6 +163,9 @@
     <t xml:space="preserve">vpilanka@uci.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">xilingl1@uci.edu</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #3 e-mail&gt;</t>
   </si>
   <si>
@@ -160,6 +181,9 @@
     <t xml:space="preserve">aman-bhatia94</t>
   </si>
   <si>
+    <t xml:space="preserve">zyjeagle</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #1 github id&gt;</t>
   </si>
   <si>
@@ -175,6 +199,9 @@
     <t xml:space="preserve">anjanakvellore</t>
   </si>
   <si>
+    <t xml:space="preserve">bingfeizh</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #2 github id&gt;</t>
   </si>
   <si>
@@ -188,6 +215,9 @@
   </si>
   <si>
     <t xml:space="preserve">vaishakhiification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xilingl1</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;member #3 github id&gt;</t>
@@ -335,13 +365,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="10"/>
@@ -362,13 +392,60 @@
       <b val="true"/>
       <sz val="16"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -380,37 +457,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="等线"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="等线"/>
-      <family val="0"/>
-      <charset val="134"/>
     </font>
     <font>
       <u val="single"/>
@@ -474,7 +520,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -484,7 +530,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -509,7 +555,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -517,7 +563,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -603,13 +657,13 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5234375" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="34.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="34.66"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -632,7 +686,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -655,11 +709,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -669,232 +723,232 @@
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
-      <c r="B5" s="6"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="B6" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="C6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>29</v>
+      <c r="A9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
+      <c r="A10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>39</v>
+      <c r="A11" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>44</v>
+        <v>50</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>54</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>60</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>54</v>
+        <v>62</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -903,7 +957,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -912,18 +966,18 @@
       <c r="F16" s="5"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -931,16 +985,16 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>75</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -949,24 +1003,24 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>79</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
@@ -974,16 +1028,16 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>73</v>
+        <v>81</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
@@ -991,101 +1045,101 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>76</v>
+        <v>30</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>80</v>
+        <v>88</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>81</v>
+        <v>91</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>84</v>
+        <v>92</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>94</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>87</v>
+        <v>48</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>97</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>91</v>
+        <v>99</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>101</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>95</v>
+        <v>103</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>105</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -1093,55 +1147,55 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>98</v>
+        <v>66</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>108</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="3" t="s">
-        <v>99</v>
+      <c r="D29" s="8" t="s">
+        <v>109</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="3" t="s">
-        <v>100</v>
+      <c r="D30" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="3" t="s">
-        <v>101</v>
+      <c r="D31" s="8" t="s">
+        <v>111</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1158,29 +1212,32 @@
     <hyperlink ref="A9" r:id="rId1" display="dongxix@uci.edu"/>
     <hyperlink ref="B9" r:id="rId2" display="andradam@uci.edu"/>
     <hyperlink ref="C9" r:id="rId3" display="amanb1@uci.edu"/>
-    <hyperlink ref="G9" r:id="rId4" display="yue.zhang@uci.edu"/>
-    <hyperlink ref="A10" r:id="rId5" display="anniejingchen@gmail.com"/>
-    <hyperlink ref="B10" r:id="rId6" display="soobinc3@uci.edu"/>
-    <hyperlink ref="C10" r:id="rId7" display="anjanak1@uci.edu"/>
-    <hyperlink ref="G10" r:id="rId8" display="zeyuh10@uci.edu"/>
-    <hyperlink ref="A11" r:id="rId9" display="guowel2@uci.edu"/>
-    <hyperlink ref="B11" r:id="rId10" display="dchai2@uci.edu"/>
-    <hyperlink ref="C11" r:id="rId11" display="vpilanka@uci.edu"/>
-    <hyperlink ref="G11" r:id="rId12" display="tianlul3@uci.edu"/>
-    <hyperlink ref="A23" r:id="rId13" display="santhiyn@uci.edu"/>
-    <hyperlink ref="B23" r:id="rId14" display="xiaoluep@uci.edu"/>
-    <hyperlink ref="C23" r:id="rId15" display="junxiac1@uci.edu"/>
-    <hyperlink ref="A24" r:id="rId16" display="shikunx@uci.edu"/>
-    <hyperlink ref="B24" r:id="rId17" display="yilin.wang@uci.edu"/>
-    <hyperlink ref="C24" r:id="rId18" display="wcyang1@uci.edu"/>
-    <hyperlink ref="D24" r:id="rId19" display="rcortezb@uci.edu"/>
-    <hyperlink ref="A25" r:id="rId20" display="yitiam2@uci.edu"/>
-    <hyperlink ref="C25" r:id="rId21" display="zihuaw2@uci.edu"/>
-    <hyperlink ref="D25" r:id="rId22" display="hjyang1@uci.edu"/>
-    <hyperlink ref="B26" r:id="rId23" display="https://github.com/gir1yaphets"/>
-    <hyperlink ref="D26" r:id="rId24" display="ngrantha@uci.edu"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://github.com/dlwangyilin"/>
-    <hyperlink ref="D27" r:id="rId26" display="czhang29@uci.edu"/>
+    <hyperlink ref="D9" r:id="rId4" display="yijiz13@uci.edu"/>
+    <hyperlink ref="G9" r:id="rId5" display="yue.zhang@uci.edu"/>
+    <hyperlink ref="A10" r:id="rId6" display="anniejingchen@gmail.com"/>
+    <hyperlink ref="B10" r:id="rId7" display="soobinc3@uci.edu"/>
+    <hyperlink ref="C10" r:id="rId8" display="anjanak1@uci.edu"/>
+    <hyperlink ref="D10" r:id="rId9" display="bingfeiz@uci.edu"/>
+    <hyperlink ref="G10" r:id="rId10" display="zeyuh10@uci.edu"/>
+    <hyperlink ref="A11" r:id="rId11" display="guowel2@uci.edu"/>
+    <hyperlink ref="B11" r:id="rId12" display="dchai2@uci.edu"/>
+    <hyperlink ref="C11" r:id="rId13" display="vpilanka@uci.edu"/>
+    <hyperlink ref="D11" r:id="rId14" display="xilingl1@uci.edu"/>
+    <hyperlink ref="G11" r:id="rId15" display="tianlul3@uci.edu"/>
+    <hyperlink ref="A23" r:id="rId16" display="santhiyn@uci.edu"/>
+    <hyperlink ref="B23" r:id="rId17" display="xiaoluep@uci.edu"/>
+    <hyperlink ref="C23" r:id="rId18" display="junxiac1@uci.edu"/>
+    <hyperlink ref="A24" r:id="rId19" display="shikunx@uci.edu"/>
+    <hyperlink ref="B24" r:id="rId20" display="yilin.wang@uci.edu"/>
+    <hyperlink ref="C24" r:id="rId21" display="wcyang1@uci.edu"/>
+    <hyperlink ref="D24" r:id="rId22" display="rcortezb@uci.edu"/>
+    <hyperlink ref="A25" r:id="rId23" display="yitiam2@uci.edu"/>
+    <hyperlink ref="C25" r:id="rId24" display="zihuaw2@uci.edu"/>
+    <hyperlink ref="D25" r:id="rId25" display="hjyang1@uci.edu"/>
+    <hyperlink ref="B26" r:id="rId26" display="https://github.com/gir1yaphets"/>
+    <hyperlink ref="D26" r:id="rId27" display="ngrantha@uci.edu"/>
+    <hyperlink ref="B27" r:id="rId28" display="https://github.com/dlwangyilin"/>
+    <hyperlink ref="D27" r:id="rId29" display="czhang29@uci.edu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Resolved Merge Conflict PR43 (#55) Close #43
* Updated diary for 'diary-thuc-nguyen.xlsx'

* added team pay4grade and modified teams.xlsx to add members

* Resolve merge conflict

Co-authored-by: Thuc Nguyen <thn079@ucsd.edu>
Co-authored-by: Kaj Dreef <kaj.dreef@gmail.com>
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="122">
   <si>
     <t xml:space="preserve">TEAMS</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">Foobar</t>
   </si>
   <si>
+    <t xml:space="preserve">pay4grade</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;team name&gt;</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t xml:space="preserve">Yijia Zhang</t>
   </si>
   <si>
+    <t xml:space="preserve">Harry Duong</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #1 name&gt;</t>
   </si>
   <si>
@@ -94,6 +100,9 @@
     <t xml:space="preserve">Bingfei Zhang</t>
   </si>
   <si>
+    <t xml:space="preserve">Deon Zhao</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #2 name&gt;</t>
   </si>
   <si>
@@ -112,6 +121,9 @@
     <t xml:space="preserve">Xiling Li</t>
   </si>
   <si>
+    <t xml:space="preserve">Thuc Nguyen</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #3 name&gt;</t>
   </si>
   <si>
@@ -130,6 +142,9 @@
     <t xml:space="preserve">yijiz13@uci.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">duonghh@gmail.com</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #1 e-mail&gt;</t>
   </si>
   <si>
@@ -148,6 +163,9 @@
     <t xml:space="preserve">bingfeiz@uci.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">chunqiz@uci.edu</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #2 e-mail&gt;</t>
   </si>
   <si>
@@ -166,6 +184,9 @@
     <t xml:space="preserve">xilingl1@uci.edu</t>
   </si>
   <si>
+    <t xml:space="preserve">thucn2@uci.edu</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #3 e-mail&gt;</t>
   </si>
   <si>
@@ -184,6 +205,9 @@
     <t xml:space="preserve">zyjeagle</t>
   </si>
   <si>
+    <t xml:space="preserve">mswe-eper</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #1 github id&gt;</t>
   </si>
   <si>
@@ -202,6 +226,9 @@
     <t xml:space="preserve">bingfeizh</t>
   </si>
   <si>
+    <t xml:space="preserve">deon9718</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;member #2 github id&gt;</t>
   </si>
   <si>
@@ -218,6 +245,9 @@
   </si>
   <si>
     <t xml:space="preserve">xilingl1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">thucnguyen95</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;member #3 github id&gt;</t>
@@ -365,13 +395,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="等线"/>
       <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -394,14 +424,7 @@
       <color rgb="FF9C0006"/>
       <name val="等线"/>
       <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -409,7 +432,47 @@
       <color rgb="FF9C5700"/>
       <name val="等线"/>
       <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="等线"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -422,28 +485,12 @@
       <i val="true"/>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="0"/>
-      <charset val="134"/>
+      <charset val="1"/>
     </font>
     <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="等线"/>
-      <family val="4"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <family val="0"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <i val="true"/>
+      <b val="true"/>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
@@ -455,7 +502,7 @@
       <sz val="12"/>
       <color rgb="FF9C5700"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -463,7 +510,7 @@
       <sz val="11"/>
       <color rgb="FF0563C1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -476,14 +523,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -496,7 +543,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -520,72 +567,76 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="2" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Excel Built-in Bad" xfId="21"/>
-    <cellStyle name="Excel Built-in Neutral" xfId="22"/>
-    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
+    <cellStyle name="Excel Built-in Neutral" xfId="20"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -655,15 +706,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="34.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="34.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="0" width="9"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -686,7 +738,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -709,7 +761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -719,20 +771,20 @@
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -741,214 +793,214 @@
       <c r="F5" s="5"/>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="D6" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="E6" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>27</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>39</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>41</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>46</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>48</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>53</v>
+        <v>59</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>62</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>59</v>
+        <v>66</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>69</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>65</v>
+        <v>73</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -957,253 +1009,1221 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>75</v>
+        <v>83</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>85</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="12"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>79</v>
+        <v>87</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>89</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>83</v>
+        <v>91</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>93</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>86</v>
+        <v>34</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>96</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>87</v>
+    <row r="23" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="7" t="s">
+        <v>97</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>90</v>
+        <v>98</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>100</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>91</v>
+    <row r="24" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="7" t="s">
+        <v>101</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>94</v>
+        <v>102</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
-        <v>95</v>
+    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="7" t="s">
+        <v>105</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>97</v>
+        <v>55</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>101</v>
+        <v>109</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" customFormat="false" ht="16.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>105</v>
+        <v>113</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>106</v>
+        <v>116</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>108</v>
+        <v>76</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>118</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="8" t="s">
-        <v>109</v>
+      <c r="D29" s="10" t="s">
+        <v>119</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="8" t="s">
-        <v>110</v>
+      <c r="D30" s="10" t="s">
+        <v>120</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="8" t="s">
-        <v>111</v>
+      <c r="D31" s="10" t="s">
+        <v>121</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="7"/>
-    </row>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="36" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="37" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="38" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="39" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="40" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="41" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="42" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="55" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="56" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="58" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="59" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="60" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="61" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="62" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="63" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="64" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="65" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="66" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="67" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="68" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="72" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="74" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="76" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="77" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="78" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="79" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="80" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="81" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="82" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="83" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="84" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="85" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="86" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="90" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="104" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="105" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="106" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="107" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="108" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="109" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="110" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="111" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="112" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="113" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="114" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="115" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="116" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="117" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="118" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="119" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="120" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="121" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="122" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="123" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="124" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="125" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="126" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="127" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="128" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="129" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="130" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="131" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="132" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="133" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="134" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="135" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="136" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="137" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="138" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="139" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="140" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="141" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="142" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="143" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="144" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="145" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="146" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="147" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="148" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="149" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="150" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="151" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="152" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="153" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="154" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="155" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="156" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="157" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="158" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="159" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="160" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="161" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="162" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="163" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="164" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="165" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="166" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="167" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="168" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="169" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="170" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="171" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="172" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="173" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="174" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="175" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="176" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="177" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="178" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="179" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="180" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="181" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="182" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="183" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="184" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="185" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="186" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="187" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="188" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="189" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="190" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="191" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="192" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="193" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="194" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="195" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="196" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="197" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="198" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="199" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="200" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="201" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="202" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="203" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="204" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="205" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="206" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="207" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="208" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="209" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="210" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="211" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="212" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="213" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="214" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="215" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="216" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="217" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="218" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="219" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="220" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="221" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="222" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="223" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="224" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="225" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="226" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="227" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="228" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="229" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="230" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="231" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="232" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="233" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="234" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="235" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="236" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="237" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="238" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="239" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="240" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="241" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="242" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="243" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="244" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="245" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="246" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="247" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="248" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="249" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="250" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="251" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="252" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="253" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="254" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="255" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="256" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="257" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="258" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="259" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="260" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="261" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="262" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="263" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="264" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="265" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="266" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="267" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="268" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="269" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="270" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="271" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="272" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="273" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="274" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="275" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="276" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="277" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="278" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="279" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="280" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="281" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="282" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="283" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="284" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="285" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="286" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="287" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="288" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="289" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="290" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="291" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="292" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="293" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="294" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="295" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="296" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="297" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="298" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="299" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="300" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="301" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="302" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="303" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="304" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="305" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="306" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="307" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="308" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="309" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="310" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="311" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="312" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="313" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="314" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="315" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="316" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="317" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="318" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="319" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="320" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="321" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="322" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="323" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="324" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="325" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="326" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="327" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="328" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="329" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="330" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="331" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="332" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="333" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="334" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="335" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="336" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="337" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="338" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="339" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="340" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="341" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="342" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="343" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="344" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="345" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="346" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="347" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="348" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="349" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="350" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="351" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="352" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="353" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="354" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="355" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="356" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="357" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="358" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="359" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="360" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="361" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="362" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="363" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="364" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="365" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="366" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="367" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="368" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="369" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="370" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="371" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="372" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="373" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="374" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="375" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="376" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="377" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="378" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="379" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="380" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="381" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="382" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="383" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="384" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="385" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="386" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="387" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="388" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="389" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="390" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="391" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="392" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="393" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="394" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="395" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="396" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="397" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="398" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="399" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="400" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="401" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="402" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="403" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="404" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="405" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="406" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="407" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="408" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="409" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="410" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="411" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="412" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="413" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="414" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="415" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="416" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="417" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="418" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="419" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="420" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="421" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="422" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="423" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="424" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="425" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="426" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="427" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="428" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="429" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="430" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="431" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="432" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="433" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="434" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="435" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="436" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="437" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="438" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="439" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="440" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="441" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="442" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="443" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="444" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="445" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="446" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="447" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="448" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="449" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="450" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="451" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="452" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="453" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="454" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="455" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="456" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="457" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="458" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="459" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="460" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="461" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="462" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="463" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="464" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="465" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="466" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="467" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="468" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="469" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="470" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="471" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="472" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="473" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="474" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="475" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="476" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="477" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="478" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="479" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="480" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="481" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="482" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="483" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="484" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="485" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="486" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="487" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="488" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="489" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="490" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="491" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="492" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="493" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="494" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="495" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="496" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="497" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="498" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="499" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="500" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="501" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="502" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="503" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="504" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="505" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="506" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="507" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="508" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="509" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="510" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="511" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="512" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="513" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="514" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="515" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="516" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="517" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="518" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="519" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="520" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="521" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="522" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="523" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="524" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="525" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="526" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="527" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="528" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="529" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="530" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="531" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="532" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="533" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="534" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="535" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="536" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="537" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="538" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="539" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="540" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="541" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="542" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="543" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="544" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="545" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="546" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="547" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="548" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="549" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="550" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="551" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="552" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="553" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="554" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="555" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="556" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="557" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="558" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="559" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="560" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="561" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="562" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="563" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="564" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="565" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="566" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="567" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="568" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="569" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="570" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="571" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="572" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="573" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="574" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="575" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="576" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="577" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="578" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="579" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="580" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="581" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="582" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="583" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="584" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="585" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="586" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="587" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="588" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="589" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="590" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="591" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="592" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="593" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="594" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="595" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="596" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="597" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="598" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="599" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="600" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="601" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="602" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="603" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="604" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="605" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="606" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="607" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="608" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="609" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="610" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="611" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="612" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="613" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="614" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="615" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="616" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="617" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="618" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="619" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="620" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="621" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="622" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="623" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="624" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="625" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="626" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="627" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="628" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="629" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="630" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="631" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="632" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="633" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="634" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="635" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="636" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="637" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="638" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="639" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="640" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="641" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="642" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="643" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="644" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="645" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="646" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="647" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="648" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="649" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="650" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="651" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="652" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="653" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="654" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="655" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="656" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="657" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="658" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="659" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="660" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="661" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="662" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="663" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="664" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="665" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="666" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="667" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="668" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="669" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="670" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="671" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="672" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="673" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="674" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="675" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="676" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="677" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="678" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="679" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="680" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="681" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="682" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="683" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="684" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="685" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="686" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="687" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="688" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="689" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="690" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="691" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="692" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="693" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="694" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="695" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="696" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="697" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="698" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="699" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="700" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="701" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="702" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="703" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="704" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="705" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="706" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="707" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="708" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="709" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="710" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="711" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="712" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="713" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="714" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="715" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="716" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="717" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="718" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="719" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="720" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="721" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="722" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="723" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="724" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="725" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="726" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="727" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="728" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="729" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="730" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="731" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="732" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="733" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="734" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="735" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="736" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="737" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="738" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="739" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="740" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="741" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="742" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="743" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="744" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="745" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="746" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="747" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="748" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="749" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="750" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="751" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="752" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="753" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="754" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="755" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="756" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="757" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="758" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="759" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="760" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="761" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="762" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="763" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="764" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="765" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="766" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="767" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="768" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="769" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="770" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="771" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="772" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="773" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="774" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="775" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="776" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="777" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="778" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="779" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="780" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="781" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="782" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="783" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="784" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="785" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="786" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="787" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="788" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="789" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="790" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="791" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="792" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="793" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="794" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="795" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="796" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="797" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="798" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="799" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="800" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="801" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="802" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="803" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="804" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="805" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="806" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="807" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="808" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="809" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="810" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="811" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="812" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="813" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="814" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="815" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="816" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="817" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="818" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="819" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="820" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="821" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="822" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="823" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="824" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="825" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="826" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="827" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="828" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="829" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="830" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="831" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="832" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="833" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="834" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="835" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="836" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="837" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="838" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="839" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="840" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="841" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="842" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="843" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="844" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="845" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="846" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="847" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="848" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="849" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="850" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="851" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="852" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="853" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="854" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="855" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="856" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="857" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="858" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="859" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="860" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="861" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="862" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="863" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="864" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="865" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="866" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="867" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="868" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="869" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="870" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="871" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="872" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="873" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="874" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="875" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="876" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="877" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="878" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="879" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="880" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="881" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="882" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="883" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="884" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="885" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="886" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="887" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="888" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="889" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="890" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="891" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="892" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="893" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="894" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="895" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="896" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="897" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="898" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="899" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="900" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="901" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="902" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="903" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="904" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="905" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="906" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="907" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="908" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="909" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="910" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="911" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="912" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="913" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="914" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="915" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="916" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="917" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="918" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="919" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="920" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="921" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="922" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="923" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="924" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="925" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="926" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="927" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="928" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="929" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="930" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="931" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="932" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="933" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="934" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="935" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="936" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="937" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="938" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="939" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="940" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="941" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="942" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="943" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="944" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="945" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="946" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="947" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="948" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="949" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="950" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="951" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="952" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="953" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="954" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="955" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="956" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="957" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="958" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="959" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="960" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="961" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="962" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="963" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="964" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="965" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="966" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="967" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="968" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="969" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="970" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="971" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="972" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="973" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="974" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="975" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="976" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="977" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="978" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="979" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="980" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="981" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="982" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="983" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="984" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="985" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="986" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="987" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="988" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="989" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="990" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="991" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="992" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="993" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="994" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="995" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="997" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="998" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="999" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1000" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:G2"/>
@@ -1213,31 +2233,34 @@
     <hyperlink ref="B9" r:id="rId2" display="andradam@uci.edu"/>
     <hyperlink ref="C9" r:id="rId3" display="amanb1@uci.edu"/>
     <hyperlink ref="D9" r:id="rId4" display="yijiz13@uci.edu"/>
-    <hyperlink ref="G9" r:id="rId5" display="yue.zhang@uci.edu"/>
-    <hyperlink ref="A10" r:id="rId6" display="anniejingchen@gmail.com"/>
-    <hyperlink ref="B10" r:id="rId7" display="soobinc3@uci.edu"/>
-    <hyperlink ref="C10" r:id="rId8" display="anjanak1@uci.edu"/>
-    <hyperlink ref="D10" r:id="rId9" display="bingfeiz@uci.edu"/>
-    <hyperlink ref="G10" r:id="rId10" display="zeyuh10@uci.edu"/>
-    <hyperlink ref="A11" r:id="rId11" display="guowel2@uci.edu"/>
-    <hyperlink ref="B11" r:id="rId12" display="dchai2@uci.edu"/>
-    <hyperlink ref="C11" r:id="rId13" display="vpilanka@uci.edu"/>
-    <hyperlink ref="D11" r:id="rId14" display="xilingl1@uci.edu"/>
-    <hyperlink ref="G11" r:id="rId15" display="tianlul3@uci.edu"/>
-    <hyperlink ref="A23" r:id="rId16" display="santhiyn@uci.edu"/>
-    <hyperlink ref="B23" r:id="rId17" display="xiaoluep@uci.edu"/>
-    <hyperlink ref="C23" r:id="rId18" display="junxiac1@uci.edu"/>
-    <hyperlink ref="A24" r:id="rId19" display="shikunx@uci.edu"/>
-    <hyperlink ref="B24" r:id="rId20" display="yilin.wang@uci.edu"/>
-    <hyperlink ref="C24" r:id="rId21" display="wcyang1@uci.edu"/>
-    <hyperlink ref="D24" r:id="rId22" display="rcortezb@uci.edu"/>
-    <hyperlink ref="A25" r:id="rId23" display="yitiam2@uci.edu"/>
-    <hyperlink ref="C25" r:id="rId24" display="zihuaw2@uci.edu"/>
-    <hyperlink ref="D25" r:id="rId25" display="hjyang1@uci.edu"/>
-    <hyperlink ref="B26" r:id="rId26" display="https://github.com/gir1yaphets"/>
-    <hyperlink ref="D26" r:id="rId27" display="ngrantha@uci.edu"/>
-    <hyperlink ref="B27" r:id="rId28" display="https://github.com/dlwangyilin"/>
-    <hyperlink ref="D27" r:id="rId29" display="czhang29@uci.edu"/>
+    <hyperlink ref="E9" r:id="rId5" display="duonghh@gmail.com"/>
+    <hyperlink ref="G9" r:id="rId6" display="yue.zhang@uci.edu"/>
+    <hyperlink ref="A10" r:id="rId7" display="anniejingchen@gmail.com"/>
+    <hyperlink ref="B10" r:id="rId8" display="soobinc3@uci.edu"/>
+    <hyperlink ref="C10" r:id="rId9" display="anjanak1@uci.edu"/>
+    <hyperlink ref="D10" r:id="rId10" display="bingfeiz@uci.edu"/>
+    <hyperlink ref="E10" r:id="rId11" display="chunqiz@uci.edu"/>
+    <hyperlink ref="G10" r:id="rId12" display="zeyuh10@uci.edu"/>
+    <hyperlink ref="A11" r:id="rId13" display="guowel2@uci.edu"/>
+    <hyperlink ref="B11" r:id="rId14" display="dchai2@uci.edu"/>
+    <hyperlink ref="C11" r:id="rId15" display="vpilanka@uci.edu"/>
+    <hyperlink ref="D11" r:id="rId16" display="xilingl1@uci.edu"/>
+    <hyperlink ref="E11" r:id="rId17" display="thucn2@uci.edu"/>
+    <hyperlink ref="G11" r:id="rId18" display="tianlul3@uci.edu"/>
+    <hyperlink ref="A23" r:id="rId19" display="santhiyn@uci.edu"/>
+    <hyperlink ref="B23" r:id="rId20" display="xiaoluep@uci.edu"/>
+    <hyperlink ref="C23" r:id="rId21" display="junxiac1@uci.edu"/>
+    <hyperlink ref="A24" r:id="rId22" display="shikunx@uci.edu"/>
+    <hyperlink ref="B24" r:id="rId23" display="yilin.wang@uci.edu"/>
+    <hyperlink ref="C24" r:id="rId24" display="wcyang1@uci.edu"/>
+    <hyperlink ref="D24" r:id="rId25" display="rcortezb@uci.edu"/>
+    <hyperlink ref="A25" r:id="rId26" display="yitiam2@uci.edu"/>
+    <hyperlink ref="C25" r:id="rId27" display="zihuaw2@uci.edu"/>
+    <hyperlink ref="D25" r:id="rId28" display="hjyang1@uci.edu"/>
+    <hyperlink ref="B26" r:id="rId29" display="https://github.com/gir1yaphets"/>
+    <hyperlink ref="D26" r:id="rId30" display="ngrantha@uci.edu"/>
+    <hyperlink ref="B27" r:id="rId31" display="https://github.com/dlwangyilin"/>
+    <hyperlink ref="D27" r:id="rId32" display="czhang29@uci.edu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Resolved Merge Conflict PR47 (#57) Close #47
* Added Team 6: Return True

* Team 6 folder

Co-authored-by: Tianyu Qi <ty.qi@hotmail.com>
Co-authored-by: Kaj Dreef <kaj.dreef@gmail.com>
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">pay4grade</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;team name&gt;</t>
+    <t xml:space="preserve">Return True</t>
   </si>
   <si>
     <t xml:space="preserve">Skateboard2Wheelchair</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">Harry Duong</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;member #1 name&gt;</t>
+    <t xml:space="preserve">Weihuan Fu</t>
   </si>
   <si>
     <t xml:space="preserve">Yue Zhang</t>
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Deon Zhao</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;member #2 name&gt;</t>
+    <t xml:space="preserve">Tianyu Qi</t>
   </si>
   <si>
     <t xml:space="preserve">Zeyu Huang</t>
@@ -145,7 +145,7 @@
     <t xml:space="preserve">duonghh@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;member #1 e-mail&gt;</t>
+    <t xml:space="preserve">tianyuq2@uci.edu</t>
   </si>
   <si>
     <t xml:space="preserve">yue.zhang@uci.edu</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">chunqiz@uci.edu</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;member #2 e-mail&gt;</t>
+    <t xml:space="preserve">weihuanf@uci.edu</t>
   </si>
   <si>
     <t xml:space="preserve">zeyuh10@uci.edu</t>
@@ -208,7 +208,7 @@
     <t xml:space="preserve">mswe-eper</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;member #1 github id&gt;</t>
+    <t xml:space="preserve"> laofuLF</t>
   </si>
   <si>
     <t xml:space="preserve">YorksonChang</t>
@@ -229,7 +229,7 @@
     <t xml:space="preserve">deon9718</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;member #2 github id&gt;</t>
+    <t xml:space="preserve">tyqi11</t>
   </si>
   <si>
     <t xml:space="preserve">Zeyuuuuuu</t>
@@ -395,7 +395,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -476,24 +476,8 @@
       <i val="true"/>
       <sz val="12"/>
       <color rgb="FF9C5700"/>
-      <name val="等线"/>
-      <family val="0"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="等线"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
@@ -576,7 +560,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -609,7 +593,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -617,15 +601,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -711,11 +687,11 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="34.66"/>
   </cols>
@@ -740,7 +716,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1002,7 +978,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1011,7 +987,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -1020,7 +996,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="7"/>
     </row>
-    <row r="17" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
         <v>78</v>
       </c>
@@ -1041,13 +1017,13 @@
       <c r="A18" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="8" t="s">
         <v>85</v>
       </c>
       <c r="E18" s="3"/>
@@ -1056,9 +1032,9 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1067,13 +1043,13 @@
       <c r="A20" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="8" t="s">
         <v>89</v>
       </c>
       <c r="E20" s="3"/>
@@ -1084,13 +1060,13 @@
       <c r="A21" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C21" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="8" t="s">
         <v>93</v>
       </c>
       <c r="E21" s="3"/>
@@ -1101,13 +1077,13 @@
       <c r="A22" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="8" t="s">
         <v>96</v>
       </c>
       <c r="E22" s="3"/>
@@ -1118,13 +1094,13 @@
       <c r="A23" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="D23" s="8" t="s">
         <v>100</v>
       </c>
       <c r="E23" s="3"/>
@@ -1135,13 +1111,13 @@
       <c r="A24" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="9" t="s">
+      <c r="C24" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="10" t="s">
         <v>104</v>
       </c>
       <c r="E24" s="3"/>
@@ -1152,13 +1128,13 @@
       <c r="A25" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C25" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="10" t="s">
         <v>107</v>
       </c>
       <c r="E25" s="3"/>
@@ -1169,13 +1145,13 @@
       <c r="A26" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="10" t="s">
         <v>111</v>
       </c>
       <c r="E26" s="3"/>
@@ -1186,13 +1162,13 @@
       <c r="A27" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C27" s="9" t="s">
+      <c r="C27" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="10" t="s">
         <v>115</v>
       </c>
       <c r="E27" s="3"/>
@@ -1203,53 +1179,53 @@
       <c r="A28" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C28" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>118</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
-      <c r="D29" s="9" t="s">
+      <c r="D29" s="8" t="s">
         <v>119</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
-      <c r="D30" s="9" t="s">
+      <c r="D30" s="8" t="s">
         <v>120</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
-      <c r="D31" s="9" t="s">
+      <c r="D31" s="8" t="s">
         <v>121</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" customFormat="false" ht="16" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="5"/>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
@@ -1268,33 +1244,35 @@
     <hyperlink ref="C9" r:id="rId3" display="amanb1@uci.edu"/>
     <hyperlink ref="D9" r:id="rId4" display="yijiz13@uci.edu"/>
     <hyperlink ref="E9" r:id="rId5" display="duonghh@gmail.com"/>
-    <hyperlink ref="G9" r:id="rId6" display="yue.zhang@uci.edu"/>
-    <hyperlink ref="A10" r:id="rId7" display="anniejingchen@gmail.com"/>
-    <hyperlink ref="B10" r:id="rId8" display="soobinc3@uci.edu"/>
-    <hyperlink ref="C10" r:id="rId9" display="anjanak1@uci.edu"/>
-    <hyperlink ref="D10" r:id="rId10" display="bingfeiz@uci.edu"/>
-    <hyperlink ref="E10" r:id="rId11" display="chunqiz@uci.edu"/>
-    <hyperlink ref="G10" r:id="rId12" display="zeyuh10@uci.edu"/>
-    <hyperlink ref="A11" r:id="rId13" display="guowel2@uci.edu"/>
-    <hyperlink ref="B11" r:id="rId14" display="dchai2@uci.edu"/>
-    <hyperlink ref="C11" r:id="rId15" display="vpilanka@uci.edu"/>
-    <hyperlink ref="D11" r:id="rId16" display="xilingl1@uci.edu"/>
-    <hyperlink ref="E11" r:id="rId17" display="thucn2@uci.edu"/>
-    <hyperlink ref="G11" r:id="rId18" display="tianlul3@uci.edu"/>
-    <hyperlink ref="A23" r:id="rId19" display="santhiyn@uci.edu"/>
-    <hyperlink ref="B23" r:id="rId20" display="xiaoluep@uci.edu"/>
-    <hyperlink ref="C23" r:id="rId21" display="junxiac1@uci.edu"/>
-    <hyperlink ref="A24" r:id="rId22" display="shikunx@uci.edu"/>
-    <hyperlink ref="B24" r:id="rId23" display="yilin.wang@uci.edu"/>
-    <hyperlink ref="C24" r:id="rId24" display="wcyang1@uci.edu"/>
-    <hyperlink ref="D24" r:id="rId25" display="rcortezb@uci.edu"/>
-    <hyperlink ref="A25" r:id="rId26" display="yitiam2@uci.edu"/>
-    <hyperlink ref="C25" r:id="rId27" display="zihuaw2@uci.edu"/>
-    <hyperlink ref="D25" r:id="rId28" display="hjyang1@uci.edu"/>
-    <hyperlink ref="B26" r:id="rId29" display="https://github.com/gir1yaphets"/>
-    <hyperlink ref="D26" r:id="rId30" display="ngrantha@uci.edu"/>
-    <hyperlink ref="B27" r:id="rId31" display="https://github.com/dlwangyilin"/>
-    <hyperlink ref="D27" r:id="rId32" display="czhang29@uci.edu"/>
+    <hyperlink ref="F9" r:id="rId6" display="tianyuq2@uci.edu"/>
+    <hyperlink ref="G9" r:id="rId7" display="yue.zhang@uci.edu"/>
+    <hyperlink ref="A10" r:id="rId8" display="anniejingchen@gmail.com"/>
+    <hyperlink ref="B10" r:id="rId9" display="soobinc3@uci.edu"/>
+    <hyperlink ref="C10" r:id="rId10" display="anjanak1@uci.edu"/>
+    <hyperlink ref="D10" r:id="rId11" display="bingfeiz@uci.edu"/>
+    <hyperlink ref="E10" r:id="rId12" display="chunqiz@uci.edu"/>
+    <hyperlink ref="F10" r:id="rId13" display="weihuanf@uci.edu"/>
+    <hyperlink ref="G10" r:id="rId14" display="zeyuh10@uci.edu"/>
+    <hyperlink ref="A11" r:id="rId15" display="guowel2@uci.edu"/>
+    <hyperlink ref="B11" r:id="rId16" display="dchai2@uci.edu"/>
+    <hyperlink ref="C11" r:id="rId17" display="vpilanka@uci.edu"/>
+    <hyperlink ref="D11" r:id="rId18" display="xilingl1@uci.edu"/>
+    <hyperlink ref="E11" r:id="rId19" display="thucn2@uci.edu"/>
+    <hyperlink ref="G11" r:id="rId20" display="tianlul3@uci.edu"/>
+    <hyperlink ref="A23" r:id="rId21" display="santhiyn@uci.edu"/>
+    <hyperlink ref="B23" r:id="rId22" display="xiaoluep@uci.edu"/>
+    <hyperlink ref="C23" r:id="rId23" display="junxiac1@uci.edu"/>
+    <hyperlink ref="A24" r:id="rId24" display="shikunx@uci.edu"/>
+    <hyperlink ref="B24" r:id="rId25" display="yilin.wang@uci.edu"/>
+    <hyperlink ref="C24" r:id="rId26" display="wcyang1@uci.edu"/>
+    <hyperlink ref="D24" r:id="rId27" display="rcortezb@uci.edu"/>
+    <hyperlink ref="A25" r:id="rId28" display="yitiam2@uci.edu"/>
+    <hyperlink ref="C25" r:id="rId29" display="zihuaw2@uci.edu"/>
+    <hyperlink ref="D25" r:id="rId30" display="hjyang1@uci.edu"/>
+    <hyperlink ref="B26" r:id="rId31" display="https://github.com/gir1yaphets"/>
+    <hyperlink ref="D26" r:id="rId32" display="ngrantha@uci.edu"/>
+    <hyperlink ref="B27" r:id="rId33" display="https://github.com/dlwangyilin"/>
+    <hyperlink ref="D27" r:id="rId34" display="czhang29@uci.edu"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Team 6 updated team members
</commit_message>
<xml_diff>
--- a/teams.xlsx
+++ b/teams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlwan\Documents\Study\reverse_engineering\W2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school\2-20_winter\265P REVERSE_ENG_&amp;_MODEL\W2020\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6E06B5-769B-4E27-857D-10022EEC3BCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F42ED856-3481-4EE4-B382-27D7DF708DD3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,9 +129,6 @@
     <t>Thuc Nguyen</t>
   </si>
   <si>
-    <t>&lt;member #3 name&gt;</t>
-  </si>
-  <si>
     <t>Tianlun Li</t>
   </si>
   <si>
@@ -192,9 +189,6 @@
     <t>thucn2@uci.edu</t>
   </si>
   <si>
-    <t>&lt;member #3 e-mail&gt;</t>
-  </si>
-  <si>
     <t>tianlul3@uci.edu</t>
   </si>
   <si>
@@ -213,9 +207,6 @@
     <t>mswe-eper</t>
   </si>
   <si>
-    <t xml:space="preserve"> laofuLF</t>
-  </si>
-  <si>
     <t>YorksonChang</t>
   </si>
   <si>
@@ -255,9 +246,6 @@
     <t>thucnguyen95</t>
   </si>
   <si>
-    <t>&lt;member #3 github id&gt;</t>
-  </si>
-  <si>
     <t>ShawnLi1014</t>
   </si>
   <si>
@@ -400,13 +388,25 @@
   </si>
   <si>
     <t>https://github.com/lindzgarcia2</t>
+  </si>
+  <si>
+    <t>Armin Hamidi </t>
+  </si>
+  <si>
+    <t>arminhamidi@outlook.com</t>
+  </si>
+  <si>
+    <t>laofuLF</t>
+  </si>
+  <si>
+    <t>ahamidi96</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -523,9 +523,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -538,12 +535,15 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Bad" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="3" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,7 +627,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -926,551 +926,551 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="7" width="34.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21" customHeight="1">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:7" ht="21" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.5">
-      <c r="A3" s="2" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:7" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.5">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="G4" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.5">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="15.5">
-      <c r="A6" s="3" t="s">
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.5">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.5">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="4" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.5">
-      <c r="A9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.5">
-      <c r="A10" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.5">
-      <c r="A11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.5">
-      <c r="A12" s="3" t="s">
+      <c r="C12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="D12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="C13" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.5">
-      <c r="A13" s="3" t="s">
+      <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="F13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="C14" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.5">
-      <c r="A14" s="3" t="s">
+      <c r="D14" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="E14" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="F14" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="B17" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="D17" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.5">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.5">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.5">
-      <c r="A17" s="2" t="s">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="D18" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.5">
-      <c r="A18" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="8" t="s">
+      <c r="D20" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.5">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.5">
-      <c r="A20" s="3" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="8" t="s">
+      <c r="D21" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.5">
-      <c r="A21" s="3" t="s">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="D22" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.5">
-      <c r="A22" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C22" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="D22" s="8" t="s">
+      <c r="D23" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.5">
-      <c r="A23" s="3" t="s">
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C24" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="8" t="s">
+      <c r="D24" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.5">
-      <c r="A24" s="3" t="s">
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B25" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D25" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.5">
-      <c r="A25" s="3" t="s">
+      <c r="B26" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="C25" s="8" t="s">
+      <c r="C26" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D26" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.5">
-      <c r="A26" s="3" t="s">
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C27" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.5">
-      <c r="A27" s="3" t="s">
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B28" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D28" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.5">
-      <c r="A28" s="3" t="s">
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B28" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="C28" s="8" t="s">
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.5">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.5">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-    </row>
-    <row r="31" spans="1:7" ht="15.5">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.5">
-      <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="7"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1482,35 +1482,33 @@
     <hyperlink ref="C9" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="D9" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="E9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="F9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="G9" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="A10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="C10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="D10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="F10" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="G10" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="A11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="B11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="C11" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="D11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E11" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="G11" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="B23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="C23" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="B24" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="C24" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="D24" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A25" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="C25" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="D25" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="B26" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="D26" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="B27" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="D27" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="G9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="C10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="D10" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E10" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G10" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A11" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="C11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="D11" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E11" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G11" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="C23" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A24" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="C24" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="D24" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A25" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="C25" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="D25" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B26" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="D26" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B27" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="D27" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>